<commit_message>
minor changes in dependenecy and updated the documentation
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenautomationlabs/Downloads/workspace/xls_reader/"/>
     </mc:Choice>
@@ -15,10 +15,11 @@
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="naveen" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -126,6 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -506,7 +508,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -530,10 +532,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -545,15 +547,15 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -565,15 +567,15 @@
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -585,15 +587,15 @@
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -605,7 +607,7 @@
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -636,4 +638,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>